<commit_message>
Macro and SaveList classes GUI work Available buttons
</commit_message>
<xml_diff>
--- a/src/test/Кнопки.xlsx
+++ b/src/test/Кнопки.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PythonProjects\EldenRing-HardSwapper\src\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22C6A1C3-DA39-40C2-B55A-337DAF6C3D06}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{522A057C-1DD0-4BF5-80A1-FF1B63ED7769}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="12804" activeTab="1" xr2:uid="{420A9529-3EEB-412F-941D-7F7F62F7DFF1}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="591" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="936" uniqueCount="187">
   <si>
     <t>Кнопка по умолчанию</t>
   </si>
@@ -578,6 +578,15 @@
   </si>
   <si>
     <t>',</t>
+  </si>
+  <si>
+    <t>("</t>
+  </si>
+  <si>
+    <t>", "</t>
+  </si>
+  <si>
+    <t>"),</t>
   </si>
 </sst>
 </file>
@@ -774,9 +783,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -831,6 +837,9 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -1319,79 +1328,79 @@
       </c>
     </row>
     <row r="14" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3" t="s">
+      <c r="D14" s="23"/>
+      <c r="E14" s="23"/>
+      <c r="F14" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
+      <c r="G14" s="23"/>
+      <c r="H14" s="23"/>
       <c r="I14" s="2"/>
-      <c r="J14" s="3" t="s">
+      <c r="J14" s="23" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B15" s="3"/>
-      <c r="C15" s="5" t="s">
+      <c r="B15" s="23"/>
+      <c r="C15" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="D15" s="6" t="s">
+      <c r="D15" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E15" s="7" t="s">
+      <c r="E15" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="F15" s="5" t="s">
+      <c r="F15" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="G15" s="6" t="s">
+      <c r="G15" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="H15" s="15" t="s">
+      <c r="H15" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="I15" s="7" t="s">
+      <c r="I15" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="J15" s="3"/>
+      <c r="J15" s="23"/>
     </row>
     <row r="16" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>30</v>
       </c>
-      <c r="C16" s="8" t="s">
+      <c r="C16" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="D16" s="9" t="s">
+      <c r="D16" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="E16" s="10" t="s">
+      <c r="E16" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="F16" s="8" t="s">
+      <c r="F16" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="G16" s="9" t="s">
+      <c r="G16" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="H16" s="16" t="s">
+      <c r="H16" s="15" t="s">
         <v>106</v>
       </c>
-      <c r="I16" s="10" t="s">
+      <c r="I16" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="J16" s="4" t="s">
+      <c r="J16" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="K16" s="4">
-        <f>H16-I16</f>
+      <c r="K16" s="3">
+        <f t="shared" ref="K16:K21" si="0">H16-I16</f>
         <v>69</v>
       </c>
     </row>
@@ -1399,32 +1408,32 @@
       <c r="B17" t="s">
         <v>31</v>
       </c>
-      <c r="C17" s="8" t="s">
+      <c r="C17" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="D17" s="9">
+      <c r="D17" s="8">
         <v>66</v>
       </c>
-      <c r="E17" s="10" t="s">
+      <c r="E17" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="F17" s="8" t="s">
+      <c r="F17" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="G17" s="9" t="s">
+      <c r="G17" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="H17" s="16" t="s">
+      <c r="H17" s="15" t="s">
         <v>107</v>
       </c>
-      <c r="I17" s="10" t="s">
+      <c r="I17" s="9" t="s">
         <v>123</v>
       </c>
-      <c r="J17" s="4" t="s">
+      <c r="J17" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="K17" s="4">
-        <f>H17-I17</f>
+      <c r="K17" s="3">
+        <f t="shared" si="0"/>
         <v>69</v>
       </c>
     </row>
@@ -1432,32 +1441,32 @@
       <c r="B18" t="s">
         <v>32</v>
       </c>
-      <c r="C18" s="8" t="s">
+      <c r="C18" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D18" s="9" t="s">
+      <c r="D18" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="E18" s="10" t="s">
+      <c r="E18" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="F18" s="8" t="s">
+      <c r="F18" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="G18" s="9" t="s">
+      <c r="G18" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="H18" s="16" t="s">
+      <c r="H18" s="15" t="s">
         <v>108</v>
       </c>
-      <c r="I18" s="10" t="s">
+      <c r="I18" s="9" t="s">
         <v>124</v>
       </c>
-      <c r="J18" s="4" t="s">
+      <c r="J18" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="K18" s="4">
-        <f>H18-I18</f>
+      <c r="K18" s="3">
+        <f t="shared" si="0"/>
         <v>69</v>
       </c>
     </row>
@@ -1465,32 +1474,32 @@
       <c r="B19" t="s">
         <v>33</v>
       </c>
-      <c r="C19" s="8" t="s">
+      <c r="C19" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D19" s="9" t="s">
+      <c r="D19" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="E19" s="10" t="s">
+      <c r="E19" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="F19" s="8">
+      <c r="F19" s="7">
         <v>6</v>
       </c>
-      <c r="G19" s="9" t="s">
+      <c r="G19" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="H19" s="16" t="s">
+      <c r="H19" s="15" t="s">
         <v>109</v>
       </c>
-      <c r="I19" s="10" t="s">
+      <c r="I19" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="J19" s="4" t="s">
+      <c r="J19" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="K19" s="4">
-        <f>H19-I19</f>
+      <c r="K19" s="3">
+        <f t="shared" si="0"/>
         <v>69</v>
       </c>
     </row>
@@ -1498,32 +1507,32 @@
       <c r="B20" t="s">
         <v>34</v>
       </c>
-      <c r="C20" s="8" t="s">
+      <c r="C20" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="D20" s="9" t="s">
+      <c r="D20" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="E20" s="10" t="s">
+      <c r="E20" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="F20" s="8" t="s">
+      <c r="F20" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="G20" s="9" t="s">
+      <c r="G20" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="H20" s="16" t="s">
+      <c r="H20" s="15" t="s">
         <v>110</v>
       </c>
-      <c r="I20" s="10" t="s">
+      <c r="I20" s="9" t="s">
         <v>126</v>
       </c>
-      <c r="J20" s="4" t="s">
+      <c r="J20" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="K20" s="4">
-        <f>H20-I20</f>
+      <c r="K20" s="3">
+        <f t="shared" si="0"/>
         <v>69</v>
       </c>
     </row>
@@ -1531,32 +1540,32 @@
       <c r="B21" t="s">
         <v>35</v>
       </c>
-      <c r="C21" s="8" t="s">
+      <c r="C21" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="D21" s="9" t="s">
+      <c r="D21" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="E21" s="10" t="s">
+      <c r="E21" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="F21" s="8" t="s">
+      <c r="F21" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="G21" s="9" t="s">
+      <c r="G21" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="H21" s="16" t="s">
+      <c r="H21" s="15" t="s">
         <v>111</v>
       </c>
-      <c r="I21" s="10" t="s">
+      <c r="I21" s="9" t="s">
         <v>127</v>
       </c>
-      <c r="J21" s="4" t="s">
+      <c r="J21" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="K21" s="4">
-        <f>H21-I21</f>
+      <c r="K21" s="3">
+        <f t="shared" si="0"/>
         <v>69</v>
       </c>
     </row>
@@ -1564,31 +1573,31 @@
       <c r="B22" t="s">
         <v>36</v>
       </c>
-      <c r="C22" s="8" t="s">
+      <c r="C22" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D22" s="9" t="s">
+      <c r="D22" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="E22" s="10" t="s">
+      <c r="E22" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="F22" s="8" t="s">
+      <c r="F22" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="G22" s="9" t="s">
+      <c r="G22" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="H22" s="18" t="s">
+      <c r="H22" s="17" t="s">
         <v>112</v>
       </c>
-      <c r="I22" s="19" t="s">
+      <c r="I22" s="18" t="s">
         <v>128</v>
       </c>
-      <c r="J22" s="4" t="s">
+      <c r="J22" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="K22" s="20">
+      <c r="K22" s="19">
         <f>140-71</f>
         <v>69</v>
       </c>
@@ -1597,31 +1606,31 @@
       <c r="B23" t="s">
         <v>37</v>
       </c>
-      <c r="C23" s="8" t="s">
+      <c r="C23" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="D23" s="9" t="s">
+      <c r="D23" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="E23" s="10" t="s">
+      <c r="E23" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="F23" s="8" t="s">
+      <c r="F23" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="G23" s="9" t="s">
+      <c r="G23" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="H23" s="16" t="s">
+      <c r="H23" s="15" t="s">
         <v>113</v>
       </c>
-      <c r="I23" s="10" t="s">
+      <c r="I23" s="9" t="s">
         <v>129</v>
       </c>
-      <c r="J23" s="4" t="s">
+      <c r="J23" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="K23" s="4">
+      <c r="K23" s="3">
         <f>H23-I23</f>
         <v>-13</v>
       </c>
@@ -1630,29 +1639,29 @@
       <c r="B24" t="s">
         <v>38</v>
       </c>
-      <c r="C24" s="8" t="s">
+      <c r="C24" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="D24" s="9" t="s">
+      <c r="D24" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="E24" s="10"/>
-      <c r="F24" s="8" t="s">
+      <c r="E24" s="9"/>
+      <c r="F24" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="G24" s="9" t="s">
+      <c r="G24" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="H24" s="16" t="s">
+      <c r="H24" s="15" t="s">
         <v>114</v>
       </c>
-      <c r="I24" s="10" t="s">
+      <c r="I24" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="J24" s="4" t="s">
+      <c r="J24" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="K24" s="4">
+      <c r="K24" s="3">
         <f>H24-I24</f>
         <v>69</v>
       </c>
@@ -1661,31 +1670,31 @@
       <c r="B25" t="s">
         <v>39</v>
       </c>
-      <c r="C25" s="8" t="s">
+      <c r="C25" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="D25" s="9" t="s">
+      <c r="D25" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="E25" s="10" t="s">
+      <c r="E25" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="F25" s="8" t="s">
+      <c r="F25" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="G25" s="9" t="s">
+      <c r="G25" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="H25" s="16" t="s">
+      <c r="H25" s="15" t="s">
         <v>115</v>
       </c>
-      <c r="I25" s="10" t="s">
+      <c r="I25" s="9" t="s">
         <v>131</v>
       </c>
-      <c r="J25" s="4" t="s">
+      <c r="J25" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="K25" s="4">
+      <c r="K25" s="3">
         <f>H25-I25</f>
         <v>19</v>
       </c>
@@ -1694,24 +1703,24 @@
       <c r="B26" t="s">
         <v>40</v>
       </c>
-      <c r="C26" s="8" t="s">
+      <c r="C26" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D26" s="9" t="s">
+      <c r="D26" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="E26" s="10" t="s">
+      <c r="E26" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="F26" s="8" t="s">
+      <c r="F26" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="G26" s="9" t="s">
+      <c r="G26" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="H26" s="16"/>
-      <c r="I26" s="10"/>
-      <c r="J26" s="4" t="s">
+      <c r="H26" s="15"/>
+      <c r="I26" s="9"/>
+      <c r="J26" s="3" t="s">
         <v>90</v>
       </c>
     </row>
@@ -1719,29 +1728,29 @@
       <c r="B27" t="s">
         <v>41</v>
       </c>
-      <c r="C27" s="11" t="s">
+      <c r="C27" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="D27" s="12" t="s">
+      <c r="D27" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="E27" s="13" t="s">
+      <c r="E27" s="12" t="s">
         <v>105</v>
       </c>
-      <c r="F27" s="11" t="s">
+      <c r="F27" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="G27" s="12" t="s">
+      <c r="G27" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="H27" s="17"/>
-      <c r="I27" s="13"/>
-      <c r="J27" s="4" t="s">
+      <c r="H27" s="16"/>
+      <c r="I27" s="12"/>
+      <c r="J27" s="3" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="29" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="F29" s="14" t="s">
+      <c r="F29" s="13" t="s">
         <v>117</v>
       </c>
     </row>
@@ -1749,11 +1758,11 @@
       <c r="B30" t="s">
         <v>116</v>
       </c>
-      <c r="D30" s="4">
+      <c r="D30" s="3">
         <f>E16-H18</f>
         <v>42</v>
       </c>
-      <c r="E30" s="14" t="s">
+      <c r="E30" s="13" t="s">
         <v>120</v>
       </c>
     </row>
@@ -1761,7 +1770,7 @@
       <c r="B31" t="s">
         <v>118</v>
       </c>
-      <c r="D31" s="4">
+      <c r="D31" s="3">
         <f>E22-E25</f>
         <v>-9</v>
       </c>
@@ -1770,7 +1779,7 @@
       <c r="B32" t="s">
         <v>119</v>
       </c>
-      <c r="D32" s="4">
+      <c r="D32" s="3">
         <f>H22-H19</f>
         <v>64</v>
       </c>
@@ -1789,15 +1798,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB02D071-5B54-4DD9-A1A6-7F738887A314}">
-  <dimension ref="A1:H74"/>
+  <dimension ref="A1:N74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:H74"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2:N74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>27</v>
       </c>
@@ -1805,11 +1814,11 @@
         <v>170</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="C2" s="22" t="s">
+    <row r="2" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="C2" s="21" t="s">
         <v>181</v>
       </c>
       <c r="D2">
@@ -1818,21 +1827,36 @@
       <c r="E2" t="s">
         <v>180</v>
       </c>
-      <c r="F2" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="G2" s="21" t="s">
+      <c r="F2" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="G2" s="20" t="s">
         <v>164</v>
       </c>
-      <c r="H2" s="23" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="C3" s="22" t="s">
+      <c r="H2" s="22" t="s">
+        <v>183</v>
+      </c>
+      <c r="J2" t="s">
+        <v>184</v>
+      </c>
+      <c r="K2" s="20" t="s">
+        <v>164</v>
+      </c>
+      <c r="L2" t="s">
+        <v>185</v>
+      </c>
+      <c r="M2" s="20" t="s">
+        <v>164</v>
+      </c>
+      <c r="N2" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="C3" s="21" t="s">
         <v>181</v>
       </c>
       <c r="D3">
@@ -1841,21 +1865,36 @@
       <c r="E3" t="s">
         <v>180</v>
       </c>
-      <c r="F3" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="G3" s="21" t="s">
+      <c r="F3" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="G3" s="20" t="s">
         <v>132</v>
       </c>
-      <c r="H3" s="23" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="C4" s="22" t="s">
+      <c r="H3" s="22" t="s">
+        <v>183</v>
+      </c>
+      <c r="J3" t="s">
+        <v>184</v>
+      </c>
+      <c r="K3" s="20" t="s">
+        <v>132</v>
+      </c>
+      <c r="L3" t="s">
+        <v>185</v>
+      </c>
+      <c r="M3" s="20" t="s">
+        <v>132</v>
+      </c>
+      <c r="N3" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="C4" s="21" t="s">
         <v>181</v>
       </c>
       <c r="D4">
@@ -1864,21 +1903,36 @@
       <c r="E4" t="s">
         <v>180</v>
       </c>
-      <c r="F4" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="G4" s="21" t="s">
+      <c r="F4" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="G4" s="20" t="s">
         <v>133</v>
       </c>
-      <c r="H4" s="23" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="C5" s="22" t="s">
+      <c r="H4" s="22" t="s">
+        <v>183</v>
+      </c>
+      <c r="J4" t="s">
+        <v>184</v>
+      </c>
+      <c r="K4" s="20" t="s">
+        <v>133</v>
+      </c>
+      <c r="L4" t="s">
+        <v>185</v>
+      </c>
+      <c r="M4" s="20" t="s">
+        <v>133</v>
+      </c>
+      <c r="N4" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="C5" s="21" t="s">
         <v>181</v>
       </c>
       <c r="D5">
@@ -1887,21 +1941,36 @@
       <c r="E5" t="s">
         <v>180</v>
       </c>
-      <c r="F5" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="G5" s="21" t="s">
+      <c r="F5" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="G5" s="20" t="s">
         <v>134</v>
       </c>
-      <c r="H5" s="23" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="C6" s="22" t="s">
+      <c r="H5" s="22" t="s">
+        <v>183</v>
+      </c>
+      <c r="J5" t="s">
+        <v>184</v>
+      </c>
+      <c r="K5" s="20" t="s">
+        <v>134</v>
+      </c>
+      <c r="L5" t="s">
+        <v>185</v>
+      </c>
+      <c r="M5" s="20" t="s">
+        <v>134</v>
+      </c>
+      <c r="N5" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="C6" s="21" t="s">
         <v>181</v>
       </c>
       <c r="D6">
@@ -1910,21 +1979,36 @@
       <c r="E6" t="s">
         <v>180</v>
       </c>
-      <c r="F6" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="G6" s="21" t="s">
+      <c r="F6" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="G6" s="20" t="s">
         <v>135</v>
       </c>
-      <c r="H6" s="23" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="C7" s="22" t="s">
+      <c r="H6" s="22" t="s">
+        <v>183</v>
+      </c>
+      <c r="J6" t="s">
+        <v>184</v>
+      </c>
+      <c r="K6" s="20" t="s">
+        <v>135</v>
+      </c>
+      <c r="L6" t="s">
+        <v>185</v>
+      </c>
+      <c r="M6" s="20" t="s">
+        <v>135</v>
+      </c>
+      <c r="N6" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="C7" s="21" t="s">
         <v>181</v>
       </c>
       <c r="D7">
@@ -1933,21 +2017,36 @@
       <c r="E7" t="s">
         <v>180</v>
       </c>
-      <c r="F7" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="G7" s="21" t="s">
+      <c r="F7" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="G7" s="20" t="s">
         <v>136</v>
       </c>
-      <c r="H7" s="23" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="C8" s="22" t="s">
+      <c r="H7" s="22" t="s">
+        <v>183</v>
+      </c>
+      <c r="J7" t="s">
+        <v>184</v>
+      </c>
+      <c r="K7" s="20" t="s">
+        <v>136</v>
+      </c>
+      <c r="L7" t="s">
+        <v>185</v>
+      </c>
+      <c r="M7" s="20" t="s">
+        <v>136</v>
+      </c>
+      <c r="N7" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="C8" s="21" t="s">
         <v>181</v>
       </c>
       <c r="D8">
@@ -1956,21 +2055,36 @@
       <c r="E8" t="s">
         <v>180</v>
       </c>
-      <c r="F8" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="G8" s="21" t="s">
+      <c r="F8" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="G8" s="20" t="s">
         <v>137</v>
       </c>
-      <c r="H8" s="23" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="C9" s="22" t="s">
+      <c r="H8" s="22" t="s">
+        <v>183</v>
+      </c>
+      <c r="J8" t="s">
+        <v>184</v>
+      </c>
+      <c r="K8" s="20" t="s">
+        <v>137</v>
+      </c>
+      <c r="L8" t="s">
+        <v>185</v>
+      </c>
+      <c r="M8" s="20" t="s">
+        <v>137</v>
+      </c>
+      <c r="N8" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="C9" s="21" t="s">
         <v>181</v>
       </c>
       <c r="D9">
@@ -1979,21 +2093,36 @@
       <c r="E9" t="s">
         <v>180</v>
       </c>
-      <c r="F9" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="G9" s="21" t="s">
+      <c r="F9" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="G9" s="20" t="s">
         <v>138</v>
       </c>
-      <c r="H9" s="23" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="C10" s="22" t="s">
+      <c r="H9" s="22" t="s">
+        <v>183</v>
+      </c>
+      <c r="J9" t="s">
+        <v>184</v>
+      </c>
+      <c r="K9" s="20" t="s">
+        <v>138</v>
+      </c>
+      <c r="L9" t="s">
+        <v>185</v>
+      </c>
+      <c r="M9" s="20" t="s">
+        <v>138</v>
+      </c>
+      <c r="N9" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="C10" s="21" t="s">
         <v>181</v>
       </c>
       <c r="D10">
@@ -2002,21 +2131,36 @@
       <c r="E10" t="s">
         <v>180</v>
       </c>
-      <c r="F10" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="G10" s="21" t="s">
+      <c r="F10" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="G10" s="20" t="s">
         <v>139</v>
       </c>
-      <c r="H10" s="23" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="C11" s="22" t="s">
+      <c r="H10" s="22" t="s">
+        <v>183</v>
+      </c>
+      <c r="J10" t="s">
+        <v>184</v>
+      </c>
+      <c r="K10" s="20" t="s">
+        <v>139</v>
+      </c>
+      <c r="L10" t="s">
+        <v>185</v>
+      </c>
+      <c r="M10" s="20" t="s">
+        <v>139</v>
+      </c>
+      <c r="N10" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="C11" s="21" t="s">
         <v>181</v>
       </c>
       <c r="D11">
@@ -2025,21 +2169,36 @@
       <c r="E11" t="s">
         <v>180</v>
       </c>
-      <c r="F11" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="G11" s="21" t="s">
+      <c r="F11" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="G11" s="20" t="s">
         <v>140</v>
       </c>
-      <c r="H11" s="23" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="C12" s="22" t="s">
+      <c r="H11" s="22" t="s">
+        <v>183</v>
+      </c>
+      <c r="J11" t="s">
+        <v>184</v>
+      </c>
+      <c r="K11" s="20" t="s">
+        <v>140</v>
+      </c>
+      <c r="L11" t="s">
+        <v>185</v>
+      </c>
+      <c r="M11" s="20" t="s">
+        <v>140</v>
+      </c>
+      <c r="N11" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="C12" s="21" t="s">
         <v>181</v>
       </c>
       <c r="D12">
@@ -2048,21 +2207,36 @@
       <c r="E12" t="s">
         <v>180</v>
       </c>
-      <c r="F12" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="G12" s="21" t="s">
+      <c r="F12" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="G12" s="20" t="s">
         <v>141</v>
       </c>
-      <c r="H12" s="23" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="C13" s="22" t="s">
+      <c r="H12" s="22" t="s">
+        <v>183</v>
+      </c>
+      <c r="J12" t="s">
+        <v>184</v>
+      </c>
+      <c r="K12" s="20" t="s">
+        <v>141</v>
+      </c>
+      <c r="L12" t="s">
+        <v>185</v>
+      </c>
+      <c r="M12" s="20" t="s">
+        <v>141</v>
+      </c>
+      <c r="N12" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="C13" s="21" t="s">
         <v>181</v>
       </c>
       <c r="D13">
@@ -2071,21 +2245,36 @@
       <c r="E13" t="s">
         <v>180</v>
       </c>
-      <c r="F13" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="G13" s="21" t="s">
+      <c r="F13" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="G13" s="20" t="s">
         <v>142</v>
       </c>
-      <c r="H13" s="23" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="C14" s="22" t="s">
+      <c r="H13" s="22" t="s">
+        <v>183</v>
+      </c>
+      <c r="J13" t="s">
+        <v>184</v>
+      </c>
+      <c r="K13" s="20" t="s">
+        <v>142</v>
+      </c>
+      <c r="L13" t="s">
+        <v>185</v>
+      </c>
+      <c r="M13" s="20" t="s">
+        <v>142</v>
+      </c>
+      <c r="N13" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="C14" s="21" t="s">
         <v>181</v>
       </c>
       <c r="D14">
@@ -2094,21 +2283,36 @@
       <c r="E14" t="s">
         <v>180</v>
       </c>
-      <c r="F14" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="G14" s="21">
+      <c r="F14" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="G14" s="20">
         <v>0</v>
       </c>
-      <c r="H14" s="23" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="C15" s="22" t="s">
+      <c r="H14" s="22" t="s">
+        <v>183</v>
+      </c>
+      <c r="J14" t="s">
+        <v>184</v>
+      </c>
+      <c r="K14" s="20">
+        <v>0</v>
+      </c>
+      <c r="L14" t="s">
+        <v>185</v>
+      </c>
+      <c r="M14" s="20">
+        <v>0</v>
+      </c>
+      <c r="N14" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="C15" s="21" t="s">
         <v>181</v>
       </c>
       <c r="D15">
@@ -2117,21 +2321,36 @@
       <c r="E15" t="s">
         <v>180</v>
       </c>
-      <c r="F15" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="G15" s="21">
+      <c r="F15" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="G15" s="20">
         <v>1</v>
       </c>
-      <c r="H15" s="23" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="C16" s="22" t="s">
+      <c r="H15" s="22" t="s">
+        <v>183</v>
+      </c>
+      <c r="J15" t="s">
+        <v>184</v>
+      </c>
+      <c r="K15" s="20">
+        <v>1</v>
+      </c>
+      <c r="L15" t="s">
+        <v>185</v>
+      </c>
+      <c r="M15" s="20">
+        <v>1</v>
+      </c>
+      <c r="N15" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="C16" s="21" t="s">
         <v>181</v>
       </c>
       <c r="D16">
@@ -2140,21 +2359,36 @@
       <c r="E16" t="s">
         <v>180</v>
       </c>
-      <c r="F16" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="G16" s="21">
+      <c r="F16" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="G16" s="20">
         <v>2</v>
       </c>
-      <c r="H16" s="23" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="C17" s="22" t="s">
+      <c r="H16" s="22" t="s">
+        <v>183</v>
+      </c>
+      <c r="J16" t="s">
+        <v>184</v>
+      </c>
+      <c r="K16" s="20">
+        <v>2</v>
+      </c>
+      <c r="L16" t="s">
+        <v>185</v>
+      </c>
+      <c r="M16" s="20">
+        <v>2</v>
+      </c>
+      <c r="N16" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="C17" s="21" t="s">
         <v>181</v>
       </c>
       <c r="D17">
@@ -2163,21 +2397,36 @@
       <c r="E17" t="s">
         <v>180</v>
       </c>
-      <c r="F17" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="G17" s="21">
+      <c r="F17" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="G17" s="20">
         <v>3</v>
       </c>
-      <c r="H17" s="23" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="C18" s="22" t="s">
+      <c r="H17" s="22" t="s">
+        <v>183</v>
+      </c>
+      <c r="J17" t="s">
+        <v>184</v>
+      </c>
+      <c r="K17" s="20">
+        <v>3</v>
+      </c>
+      <c r="L17" t="s">
+        <v>185</v>
+      </c>
+      <c r="M17" s="20">
+        <v>3</v>
+      </c>
+      <c r="N17" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="C18" s="21" t="s">
         <v>181</v>
       </c>
       <c r="D18">
@@ -2186,21 +2435,36 @@
       <c r="E18" t="s">
         <v>180</v>
       </c>
-      <c r="F18" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="G18" s="21">
+      <c r="F18" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="G18" s="20">
         <v>4</v>
       </c>
-      <c r="H18" s="23" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="C19" s="22" t="s">
+      <c r="H18" s="22" t="s">
+        <v>183</v>
+      </c>
+      <c r="J18" t="s">
+        <v>184</v>
+      </c>
+      <c r="K18" s="20">
+        <v>4</v>
+      </c>
+      <c r="L18" t="s">
+        <v>185</v>
+      </c>
+      <c r="M18" s="20">
+        <v>4</v>
+      </c>
+      <c r="N18" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="C19" s="21" t="s">
         <v>181</v>
       </c>
       <c r="D19">
@@ -2209,21 +2473,36 @@
       <c r="E19" t="s">
         <v>180</v>
       </c>
-      <c r="F19" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="G19" s="21">
+      <c r="F19" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="G19" s="20">
         <v>5</v>
       </c>
-      <c r="H19" s="23" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="C20" s="22" t="s">
+      <c r="H19" s="22" t="s">
+        <v>183</v>
+      </c>
+      <c r="J19" t="s">
+        <v>184</v>
+      </c>
+      <c r="K19" s="20">
+        <v>5</v>
+      </c>
+      <c r="L19" t="s">
+        <v>185</v>
+      </c>
+      <c r="M19" s="20">
+        <v>5</v>
+      </c>
+      <c r="N19" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="C20" s="21" t="s">
         <v>181</v>
       </c>
       <c r="D20">
@@ -2232,21 +2511,36 @@
       <c r="E20" t="s">
         <v>180</v>
       </c>
-      <c r="F20" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="G20" s="21">
+      <c r="F20" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="G20" s="20">
         <v>6</v>
       </c>
-      <c r="H20" s="23" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="C21" s="22" t="s">
+      <c r="H20" s="22" t="s">
+        <v>183</v>
+      </c>
+      <c r="J20" t="s">
+        <v>184</v>
+      </c>
+      <c r="K20" s="20">
+        <v>6</v>
+      </c>
+      <c r="L20" t="s">
+        <v>185</v>
+      </c>
+      <c r="M20" s="20">
+        <v>6</v>
+      </c>
+      <c r="N20" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="C21" s="21" t="s">
         <v>181</v>
       </c>
       <c r="D21">
@@ -2255,21 +2549,36 @@
       <c r="E21" t="s">
         <v>180</v>
       </c>
-      <c r="F21" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="G21" s="21">
+      <c r="F21" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="G21" s="20">
         <v>7</v>
       </c>
-      <c r="H21" s="23" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="C22" s="22" t="s">
+      <c r="H21" s="22" t="s">
+        <v>183</v>
+      </c>
+      <c r="J21" t="s">
+        <v>184</v>
+      </c>
+      <c r="K21" s="20">
+        <v>7</v>
+      </c>
+      <c r="L21" t="s">
+        <v>185</v>
+      </c>
+      <c r="M21" s="20">
+        <v>7</v>
+      </c>
+      <c r="N21" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="C22" s="21" t="s">
         <v>181</v>
       </c>
       <c r="D22">
@@ -2278,21 +2587,36 @@
       <c r="E22" t="s">
         <v>180</v>
       </c>
-      <c r="F22" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="G22" s="21">
+      <c r="F22" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="G22" s="20">
         <v>8</v>
       </c>
-      <c r="H22" s="23" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="C23" s="22" t="s">
+      <c r="H22" s="22" t="s">
+        <v>183</v>
+      </c>
+      <c r="J22" t="s">
+        <v>184</v>
+      </c>
+      <c r="K22" s="20">
+        <v>8</v>
+      </c>
+      <c r="L22" t="s">
+        <v>185</v>
+      </c>
+      <c r="M22" s="20">
+        <v>8</v>
+      </c>
+      <c r="N22" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="C23" s="21" t="s">
         <v>181</v>
       </c>
       <c r="D23">
@@ -2301,21 +2625,36 @@
       <c r="E23" t="s">
         <v>180</v>
       </c>
-      <c r="F23" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="G23" s="21">
+      <c r="F23" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="G23" s="20">
         <v>9</v>
       </c>
-      <c r="H23" s="23" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="C24" s="22" t="s">
+      <c r="H23" s="22" t="s">
+        <v>183</v>
+      </c>
+      <c r="J23" t="s">
+        <v>184</v>
+      </c>
+      <c r="K23" s="20">
+        <v>9</v>
+      </c>
+      <c r="L23" t="s">
+        <v>185</v>
+      </c>
+      <c r="M23" s="20">
+        <v>9</v>
+      </c>
+      <c r="N23" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="C24" s="21" t="s">
         <v>181</v>
       </c>
       <c r="D24">
@@ -2324,21 +2663,36 @@
       <c r="E24" t="s">
         <v>180</v>
       </c>
-      <c r="F24" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="G24" s="21" t="s">
+      <c r="F24" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="G24" s="20" t="s">
         <v>171</v>
       </c>
-      <c r="H24" s="23" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="C25" s="22" t="s">
+      <c r="H24" s="22" t="s">
+        <v>183</v>
+      </c>
+      <c r="J24" t="s">
+        <v>184</v>
+      </c>
+      <c r="K24" s="20" t="s">
+        <v>171</v>
+      </c>
+      <c r="L24" t="s">
+        <v>185</v>
+      </c>
+      <c r="M24" s="20" t="s">
+        <v>171</v>
+      </c>
+      <c r="N24" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="C25" s="21" t="s">
         <v>181</v>
       </c>
       <c r="D25">
@@ -2347,21 +2701,36 @@
       <c r="E25" t="s">
         <v>180</v>
       </c>
-      <c r="F25" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="G25" s="21" t="s">
+      <c r="F25" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="G25" s="20" t="s">
         <v>172</v>
       </c>
-      <c r="H25" s="23" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="C26" s="22" t="s">
+      <c r="H25" s="22" t="s">
+        <v>183</v>
+      </c>
+      <c r="J25" t="s">
+        <v>184</v>
+      </c>
+      <c r="K25" s="20" t="s">
+        <v>172</v>
+      </c>
+      <c r="L25" t="s">
+        <v>185</v>
+      </c>
+      <c r="M25" s="20" t="s">
+        <v>172</v>
+      </c>
+      <c r="N25" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="C26" s="21" t="s">
         <v>181</v>
       </c>
       <c r="D26">
@@ -2370,21 +2739,36 @@
       <c r="E26" t="s">
         <v>180</v>
       </c>
-      <c r="F26" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="G26" s="21" t="s">
+      <c r="F26" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="G26" s="20" t="s">
         <v>173</v>
       </c>
-      <c r="H26" s="23" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="C27" s="22" t="s">
+      <c r="H26" s="22" t="s">
+        <v>183</v>
+      </c>
+      <c r="J26" t="s">
+        <v>184</v>
+      </c>
+      <c r="K26" s="20" t="s">
+        <v>173</v>
+      </c>
+      <c r="L26" t="s">
+        <v>185</v>
+      </c>
+      <c r="M26" s="20" t="s">
+        <v>173</v>
+      </c>
+      <c r="N26" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="C27" s="21" t="s">
         <v>181</v>
       </c>
       <c r="D27">
@@ -2393,21 +2777,36 @@
       <c r="E27" t="s">
         <v>180</v>
       </c>
-      <c r="F27" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="G27" s="21" t="s">
+      <c r="F27" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="G27" s="20" t="s">
         <v>174</v>
       </c>
-      <c r="H27" s="23" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="C28" s="22" t="s">
+      <c r="H27" s="22" t="s">
+        <v>183</v>
+      </c>
+      <c r="J27" t="s">
+        <v>184</v>
+      </c>
+      <c r="K27" s="20" t="s">
+        <v>174</v>
+      </c>
+      <c r="L27" t="s">
+        <v>185</v>
+      </c>
+      <c r="M27" s="20" t="s">
+        <v>174</v>
+      </c>
+      <c r="N27" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="C28" s="21" t="s">
         <v>181</v>
       </c>
       <c r="D28">
@@ -2416,21 +2815,36 @@
       <c r="E28" t="s">
         <v>180</v>
       </c>
-      <c r="F28" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="G28" s="21" t="s">
+      <c r="F28" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="G28" s="20" t="s">
         <v>175</v>
       </c>
-      <c r="H28" s="23" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="C29" s="22" t="s">
+      <c r="H28" s="22" t="s">
+        <v>183</v>
+      </c>
+      <c r="J28" t="s">
+        <v>184</v>
+      </c>
+      <c r="K28" s="20" t="s">
+        <v>175</v>
+      </c>
+      <c r="L28" t="s">
+        <v>185</v>
+      </c>
+      <c r="M28" s="20" t="s">
+        <v>175</v>
+      </c>
+      <c r="N28" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="C29" s="21" t="s">
         <v>181</v>
       </c>
       <c r="D29">
@@ -2439,21 +2853,36 @@
       <c r="E29" t="s">
         <v>180</v>
       </c>
-      <c r="F29" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="G29" s="21" t="s">
+      <c r="F29" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="G29" s="20" t="s">
         <v>176</v>
       </c>
-      <c r="H29" s="23" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="C30" s="22" t="s">
+      <c r="H29" s="22" t="s">
+        <v>183</v>
+      </c>
+      <c r="J29" t="s">
+        <v>184</v>
+      </c>
+      <c r="K29" s="20" t="s">
+        <v>176</v>
+      </c>
+      <c r="L29" t="s">
+        <v>185</v>
+      </c>
+      <c r="M29" s="20" t="s">
+        <v>176</v>
+      </c>
+      <c r="N29" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="C30" s="21" t="s">
         <v>181</v>
       </c>
       <c r="D30">
@@ -2462,21 +2891,36 @@
       <c r="E30" t="s">
         <v>180</v>
       </c>
-      <c r="F30" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="G30" s="21" t="s">
+      <c r="F30" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="G30" s="20" t="s">
         <v>177</v>
       </c>
-      <c r="H30" s="23" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="C31" s="22" t="s">
+      <c r="H30" s="22" t="s">
+        <v>183</v>
+      </c>
+      <c r="J30" t="s">
+        <v>184</v>
+      </c>
+      <c r="K30" s="20" t="s">
+        <v>177</v>
+      </c>
+      <c r="L30" t="s">
+        <v>185</v>
+      </c>
+      <c r="M30" s="20" t="s">
+        <v>177</v>
+      </c>
+      <c r="N30" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="C31" s="21" t="s">
         <v>181</v>
       </c>
       <c r="D31">
@@ -2485,21 +2929,36 @@
       <c r="E31" t="s">
         <v>180</v>
       </c>
-      <c r="F31" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="G31" s="21" t="s">
+      <c r="F31" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="G31" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="H31" s="23" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="C32" s="22" t="s">
+      <c r="H31" s="22" t="s">
+        <v>183</v>
+      </c>
+      <c r="J31" t="s">
+        <v>184</v>
+      </c>
+      <c r="K31" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="L31" t="s">
+        <v>185</v>
+      </c>
+      <c r="M31" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="N31" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="C32" s="21" t="s">
         <v>181</v>
       </c>
       <c r="D32">
@@ -2508,21 +2967,36 @@
       <c r="E32" t="s">
         <v>180</v>
       </c>
-      <c r="F32" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="G32" s="21" t="s">
+      <c r="F32" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="G32" s="20" t="s">
         <v>178</v>
       </c>
-      <c r="H32" s="23" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="C33" s="22" t="s">
+      <c r="H32" s="22" t="s">
+        <v>183</v>
+      </c>
+      <c r="J32" t="s">
+        <v>184</v>
+      </c>
+      <c r="K32" s="20" t="s">
+        <v>178</v>
+      </c>
+      <c r="L32" t="s">
+        <v>185</v>
+      </c>
+      <c r="M32" s="20" t="s">
+        <v>178</v>
+      </c>
+      <c r="N32" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="C33" s="21" t="s">
         <v>181</v>
       </c>
       <c r="D33">
@@ -2531,21 +3005,36 @@
       <c r="E33" t="s">
         <v>180</v>
       </c>
-      <c r="F33" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="G33" s="21" t="s">
+      <c r="F33" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="G33" s="20" t="s">
         <v>179</v>
       </c>
-      <c r="H33" s="23" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="C34" s="22" t="s">
+      <c r="H33" s="22" t="s">
+        <v>183</v>
+      </c>
+      <c r="J33" t="s">
+        <v>184</v>
+      </c>
+      <c r="K33" s="20" t="s">
+        <v>179</v>
+      </c>
+      <c r="L33" t="s">
+        <v>185</v>
+      </c>
+      <c r="M33" s="20" t="s">
+        <v>179</v>
+      </c>
+      <c r="N33" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="C34" s="21" t="s">
         <v>181</v>
       </c>
       <c r="D34">
@@ -2554,21 +3043,36 @@
       <c r="E34" t="s">
         <v>180</v>
       </c>
-      <c r="F34" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="G34" s="21" t="s">
+      <c r="F34" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="G34" s="20" t="s">
         <v>143</v>
       </c>
-      <c r="H34" s="23" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="C35" s="22" t="s">
+      <c r="H34" s="22" t="s">
+        <v>183</v>
+      </c>
+      <c r="J34" t="s">
+        <v>184</v>
+      </c>
+      <c r="K34" s="20" t="s">
+        <v>143</v>
+      </c>
+      <c r="L34" t="s">
+        <v>185</v>
+      </c>
+      <c r="M34" s="20" t="s">
+        <v>143</v>
+      </c>
+      <c r="N34" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="C35" s="21" t="s">
         <v>181</v>
       </c>
       <c r="D35">
@@ -2577,21 +3081,36 @@
       <c r="E35" t="s">
         <v>180</v>
       </c>
-      <c r="F35" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="G35" s="21" t="s">
+      <c r="F35" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="G35" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="H35" s="23" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="C36" s="22" t="s">
+      <c r="H35" s="22" t="s">
+        <v>183</v>
+      </c>
+      <c r="J35" t="s">
+        <v>184</v>
+      </c>
+      <c r="K35" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="L35" t="s">
+        <v>185</v>
+      </c>
+      <c r="M35" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="N35" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="C36" s="21" t="s">
         <v>181</v>
       </c>
       <c r="D36">
@@ -2600,21 +3119,36 @@
       <c r="E36" t="s">
         <v>180</v>
       </c>
-      <c r="F36" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="G36" s="21" t="s">
+      <c r="F36" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="G36" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="H36" s="23" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="C37" s="22" t="s">
+      <c r="H36" s="22" t="s">
+        <v>183</v>
+      </c>
+      <c r="J36" t="s">
+        <v>184</v>
+      </c>
+      <c r="K36" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="L36" t="s">
+        <v>185</v>
+      </c>
+      <c r="M36" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="N36" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="C37" s="21" t="s">
         <v>181</v>
       </c>
       <c r="D37">
@@ -2623,21 +3157,36 @@
       <c r="E37" t="s">
         <v>180</v>
       </c>
-      <c r="F37" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="G37" s="21" t="s">
+      <c r="F37" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="G37" s="20" t="s">
         <v>144</v>
       </c>
-      <c r="H37" s="23" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="C38" s="22" t="s">
+      <c r="H37" s="22" t="s">
+        <v>183</v>
+      </c>
+      <c r="J37" t="s">
+        <v>184</v>
+      </c>
+      <c r="K37" s="20" t="s">
+        <v>144</v>
+      </c>
+      <c r="L37" t="s">
+        <v>185</v>
+      </c>
+      <c r="M37" s="20" t="s">
+        <v>144</v>
+      </c>
+      <c r="N37" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="C38" s="21" t="s">
         <v>181</v>
       </c>
       <c r="D38">
@@ -2646,21 +3195,36 @@
       <c r="E38" t="s">
         <v>180</v>
       </c>
-      <c r="F38" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="G38" s="21" t="s">
+      <c r="F38" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="G38" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="H38" s="23" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="C39" s="22" t="s">
+      <c r="H38" s="22" t="s">
+        <v>183</v>
+      </c>
+      <c r="J38" t="s">
+        <v>184</v>
+      </c>
+      <c r="K38" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="L38" t="s">
+        <v>185</v>
+      </c>
+      <c r="M38" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="N38" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="C39" s="21" t="s">
         <v>181</v>
       </c>
       <c r="D39">
@@ -2669,21 +3233,36 @@
       <c r="E39" t="s">
         <v>180</v>
       </c>
-      <c r="F39" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="G39" s="21" t="s">
+      <c r="F39" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="G39" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="H39" s="23" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="C40" s="22" t="s">
+      <c r="H39" s="22" t="s">
+        <v>183</v>
+      </c>
+      <c r="J39" t="s">
+        <v>184</v>
+      </c>
+      <c r="K39" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="L39" t="s">
+        <v>185</v>
+      </c>
+      <c r="M39" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="N39" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="C40" s="21" t="s">
         <v>181</v>
       </c>
       <c r="D40">
@@ -2692,21 +3271,36 @@
       <c r="E40" t="s">
         <v>180</v>
       </c>
-      <c r="F40" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="G40" s="21" t="s">
+      <c r="F40" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="G40" s="20" t="s">
         <v>145</v>
       </c>
-      <c r="H40" s="23" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="C41" s="22" t="s">
+      <c r="H40" s="22" t="s">
+        <v>183</v>
+      </c>
+      <c r="J40" t="s">
+        <v>184</v>
+      </c>
+      <c r="K40" s="20" t="s">
+        <v>145</v>
+      </c>
+      <c r="L40" t="s">
+        <v>185</v>
+      </c>
+      <c r="M40" s="20" t="s">
+        <v>145</v>
+      </c>
+      <c r="N40" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="C41" s="21" t="s">
         <v>181</v>
       </c>
       <c r="D41">
@@ -2715,21 +3309,36 @@
       <c r="E41" t="s">
         <v>180</v>
       </c>
-      <c r="F41" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="G41" s="21" t="s">
+      <c r="F41" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="G41" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="H41" s="23" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="C42" s="22" t="s">
+      <c r="H41" s="22" t="s">
+        <v>183</v>
+      </c>
+      <c r="J41" t="s">
+        <v>184</v>
+      </c>
+      <c r="K41" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="L41" t="s">
+        <v>185</v>
+      </c>
+      <c r="M41" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="N41" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A42" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="C42" s="21" t="s">
         <v>181</v>
       </c>
       <c r="D42">
@@ -2738,21 +3347,36 @@
       <c r="E42" t="s">
         <v>180</v>
       </c>
-      <c r="F42" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="G42" s="21" t="s">
+      <c r="F42" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="G42" s="20" t="s">
         <v>146</v>
       </c>
-      <c r="H42" s="23" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="C43" s="22" t="s">
+      <c r="H42" s="22" t="s">
+        <v>183</v>
+      </c>
+      <c r="J42" t="s">
+        <v>184</v>
+      </c>
+      <c r="K42" s="20" t="s">
+        <v>146</v>
+      </c>
+      <c r="L42" t="s">
+        <v>185</v>
+      </c>
+      <c r="M42" s="20" t="s">
+        <v>146</v>
+      </c>
+      <c r="N42" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="C43" s="21" t="s">
         <v>181</v>
       </c>
       <c r="D43">
@@ -2761,21 +3385,36 @@
       <c r="E43" t="s">
         <v>180</v>
       </c>
-      <c r="F43" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="G43" s="21" t="s">
+      <c r="F43" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="G43" s="20" t="s">
         <v>147</v>
       </c>
-      <c r="H43" s="23" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="C44" s="22" t="s">
+      <c r="H43" s="22" t="s">
+        <v>183</v>
+      </c>
+      <c r="J43" t="s">
+        <v>184</v>
+      </c>
+      <c r="K43" s="20" t="s">
+        <v>147</v>
+      </c>
+      <c r="L43" t="s">
+        <v>185</v>
+      </c>
+      <c r="M43" s="20" t="s">
+        <v>147</v>
+      </c>
+      <c r="N43" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A44" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="C44" s="21" t="s">
         <v>181</v>
       </c>
       <c r="D44">
@@ -2784,21 +3423,36 @@
       <c r="E44" t="s">
         <v>180</v>
       </c>
-      <c r="F44" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="G44" s="21" t="s">
+      <c r="F44" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="G44" s="20" t="s">
         <v>148</v>
       </c>
-      <c r="H44" s="23" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="C45" s="22" t="s">
+      <c r="H44" s="22" t="s">
+        <v>183</v>
+      </c>
+      <c r="J44" t="s">
+        <v>184</v>
+      </c>
+      <c r="K44" s="20" t="s">
+        <v>148</v>
+      </c>
+      <c r="L44" t="s">
+        <v>185</v>
+      </c>
+      <c r="M44" s="20" t="s">
+        <v>148</v>
+      </c>
+      <c r="N44" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="C45" s="21" t="s">
         <v>181</v>
       </c>
       <c r="D45">
@@ -2807,21 +3461,36 @@
       <c r="E45" t="s">
         <v>180</v>
       </c>
-      <c r="F45" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="G45" s="21" t="s">
+      <c r="F45" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="G45" s="20" t="s">
         <v>149</v>
       </c>
-      <c r="H45" s="23" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="C46" s="22" t="s">
+      <c r="H45" s="22" t="s">
+        <v>183</v>
+      </c>
+      <c r="J45" t="s">
+        <v>184</v>
+      </c>
+      <c r="K45" s="20" t="s">
+        <v>149</v>
+      </c>
+      <c r="L45" t="s">
+        <v>185</v>
+      </c>
+      <c r="M45" s="20" t="s">
+        <v>149</v>
+      </c>
+      <c r="N45" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="C46" s="21" t="s">
         <v>181</v>
       </c>
       <c r="D46">
@@ -2830,21 +3499,36 @@
       <c r="E46" t="s">
         <v>180</v>
       </c>
-      <c r="F46" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="G46" s="21" t="s">
+      <c r="F46" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="G46" s="20" t="s">
         <v>150</v>
       </c>
-      <c r="H46" s="23" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="C47" s="22" t="s">
+      <c r="H46" s="22" t="s">
+        <v>183</v>
+      </c>
+      <c r="J46" t="s">
+        <v>184</v>
+      </c>
+      <c r="K46" s="20" t="s">
+        <v>150</v>
+      </c>
+      <c r="L46" t="s">
+        <v>185</v>
+      </c>
+      <c r="M46" s="20" t="s">
+        <v>150</v>
+      </c>
+      <c r="N46" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A47" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="C47" s="21" t="s">
         <v>181</v>
       </c>
       <c r="D47">
@@ -2853,21 +3537,36 @@
       <c r="E47" t="s">
         <v>180</v>
       </c>
-      <c r="F47" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="G47" s="21" t="s">
+      <c r="F47" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="G47" s="20" t="s">
         <v>151</v>
       </c>
-      <c r="H47" s="23" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="C48" s="22" t="s">
+      <c r="H47" s="22" t="s">
+        <v>183</v>
+      </c>
+      <c r="J47" t="s">
+        <v>184</v>
+      </c>
+      <c r="K47" s="20" t="s">
+        <v>151</v>
+      </c>
+      <c r="L47" t="s">
+        <v>185</v>
+      </c>
+      <c r="M47" s="20" t="s">
+        <v>151</v>
+      </c>
+      <c r="N47" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A48" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="C48" s="21" t="s">
         <v>181</v>
       </c>
       <c r="D48">
@@ -2876,21 +3575,36 @@
       <c r="E48" t="s">
         <v>180</v>
       </c>
-      <c r="F48" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="G48" s="21" t="s">
+      <c r="F48" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="G48" s="20" t="s">
         <v>152</v>
       </c>
-      <c r="H48" s="23" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="C49" s="22" t="s">
+      <c r="H48" s="22" t="s">
+        <v>183</v>
+      </c>
+      <c r="J48" t="s">
+        <v>184</v>
+      </c>
+      <c r="K48" s="20" t="s">
+        <v>152</v>
+      </c>
+      <c r="L48" t="s">
+        <v>185</v>
+      </c>
+      <c r="M48" s="20" t="s">
+        <v>152</v>
+      </c>
+      <c r="N48" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A49" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="C49" s="21" t="s">
         <v>181</v>
       </c>
       <c r="D49">
@@ -2899,21 +3613,36 @@
       <c r="E49" t="s">
         <v>180</v>
       </c>
-      <c r="F49" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="G49" s="21" t="s">
+      <c r="F49" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="G49" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="H49" s="23" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="C50" s="22" t="s">
+      <c r="H49" s="22" t="s">
+        <v>183</v>
+      </c>
+      <c r="J49" t="s">
+        <v>184</v>
+      </c>
+      <c r="K49" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="L49" t="s">
+        <v>185</v>
+      </c>
+      <c r="M49" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="N49" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A50" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="C50" s="21" t="s">
         <v>181</v>
       </c>
       <c r="D50">
@@ -2922,21 +3651,36 @@
       <c r="E50" t="s">
         <v>180</v>
       </c>
-      <c r="F50" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="G50" s="21" t="s">
+      <c r="F50" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="G50" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="H50" s="23" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A51" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="C51" s="22" t="s">
+      <c r="H50" s="22" t="s">
+        <v>183</v>
+      </c>
+      <c r="J50" t="s">
+        <v>184</v>
+      </c>
+      <c r="K50" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="L50" t="s">
+        <v>185</v>
+      </c>
+      <c r="M50" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="N50" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A51" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="C51" s="21" t="s">
         <v>181</v>
       </c>
       <c r="D51">
@@ -2945,21 +3689,36 @@
       <c r="E51" t="s">
         <v>180</v>
       </c>
-      <c r="F51" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="G51" s="21" t="s">
+      <c r="F51" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="G51" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="H51" s="23" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="C52" s="22" t="s">
+      <c r="H51" s="22" t="s">
+        <v>183</v>
+      </c>
+      <c r="J51" t="s">
+        <v>184</v>
+      </c>
+      <c r="K51" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="L51" t="s">
+        <v>185</v>
+      </c>
+      <c r="M51" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="N51" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A52" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="C52" s="21" t="s">
         <v>181</v>
       </c>
       <c r="D52">
@@ -2968,21 +3727,36 @@
       <c r="E52" t="s">
         <v>180</v>
       </c>
-      <c r="F52" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="G52" s="21" t="s">
+      <c r="F52" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="G52" s="20" t="s">
         <v>153</v>
       </c>
-      <c r="H52" s="23" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A53" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="C53" s="22" t="s">
+      <c r="H52" s="22" t="s">
+        <v>183</v>
+      </c>
+      <c r="J52" t="s">
+        <v>184</v>
+      </c>
+      <c r="K52" s="20" t="s">
+        <v>153</v>
+      </c>
+      <c r="L52" t="s">
+        <v>185</v>
+      </c>
+      <c r="M52" s="20" t="s">
+        <v>153</v>
+      </c>
+      <c r="N52" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A53" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="C53" s="21" t="s">
         <v>181</v>
       </c>
       <c r="D53">
@@ -2991,21 +3765,36 @@
       <c r="E53" t="s">
         <v>180</v>
       </c>
-      <c r="F53" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="G53" s="21" t="s">
+      <c r="F53" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="G53" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="H53" s="23" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A54" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="C54" s="22" t="s">
+      <c r="H53" s="22" t="s">
+        <v>183</v>
+      </c>
+      <c r="J53" t="s">
+        <v>184</v>
+      </c>
+      <c r="K53" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="L53" t="s">
+        <v>185</v>
+      </c>
+      <c r="M53" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="N53" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A54" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="C54" s="21" t="s">
         <v>181</v>
       </c>
       <c r="D54">
@@ -3014,21 +3803,36 @@
       <c r="E54" t="s">
         <v>180</v>
       </c>
-      <c r="F54" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="G54" s="21" t="s">
+      <c r="F54" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="G54" s="20" t="s">
         <v>154</v>
       </c>
-      <c r="H54" s="23" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="C55" s="22" t="s">
+      <c r="H54" s="22" t="s">
+        <v>183</v>
+      </c>
+      <c r="J54" t="s">
+        <v>184</v>
+      </c>
+      <c r="K54" s="20" t="s">
+        <v>154</v>
+      </c>
+      <c r="L54" t="s">
+        <v>185</v>
+      </c>
+      <c r="M54" s="20" t="s">
+        <v>154</v>
+      </c>
+      <c r="N54" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A55" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="C55" s="21" t="s">
         <v>181</v>
       </c>
       <c r="D55">
@@ -3037,21 +3841,36 @@
       <c r="E55" t="s">
         <v>180</v>
       </c>
-      <c r="F55" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="G55" s="21" t="s">
+      <c r="F55" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="G55" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="H55" s="23" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A56" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="C56" s="22" t="s">
+      <c r="H55" s="22" t="s">
+        <v>183</v>
+      </c>
+      <c r="J55" t="s">
+        <v>184</v>
+      </c>
+      <c r="K55" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="L55" t="s">
+        <v>185</v>
+      </c>
+      <c r="M55" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="N55" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A56" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="C56" s="21" t="s">
         <v>181</v>
       </c>
       <c r="D56">
@@ -3060,21 +3879,36 @@
       <c r="E56" t="s">
         <v>180</v>
       </c>
-      <c r="F56" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="G56" s="21" t="s">
+      <c r="F56" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="G56" s="20" t="s">
         <v>155</v>
       </c>
-      <c r="H56" s="23" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A57" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="C57" s="22" t="s">
+      <c r="H56" s="22" t="s">
+        <v>183</v>
+      </c>
+      <c r="J56" t="s">
+        <v>184</v>
+      </c>
+      <c r="K56" s="20" t="s">
+        <v>155</v>
+      </c>
+      <c r="L56" t="s">
+        <v>185</v>
+      </c>
+      <c r="M56" s="20" t="s">
+        <v>155</v>
+      </c>
+      <c r="N56" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="57" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A57" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="C57" s="21" t="s">
         <v>181</v>
       </c>
       <c r="D57">
@@ -3083,21 +3917,36 @@
       <c r="E57" t="s">
         <v>180</v>
       </c>
-      <c r="F57" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="G57" s="21" t="s">
+      <c r="F57" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="G57" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="H57" s="23" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A58" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="C58" s="22" t="s">
+      <c r="H57" s="22" t="s">
+        <v>183</v>
+      </c>
+      <c r="J57" t="s">
+        <v>184</v>
+      </c>
+      <c r="K57" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="L57" t="s">
+        <v>185</v>
+      </c>
+      <c r="M57" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="N57" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A58" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="C58" s="21" t="s">
         <v>181</v>
       </c>
       <c r="D58">
@@ -3106,21 +3955,36 @@
       <c r="E58" t="s">
         <v>180</v>
       </c>
-      <c r="F58" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="G58" s="21" t="s">
+      <c r="F58" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="G58" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="H58" s="23" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A59" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="C59" s="22" t="s">
+      <c r="H58" s="22" t="s">
+        <v>183</v>
+      </c>
+      <c r="J58" t="s">
+        <v>184</v>
+      </c>
+      <c r="K58" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="L58" t="s">
+        <v>185</v>
+      </c>
+      <c r="M58" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="N58" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="59" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A59" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="C59" s="21" t="s">
         <v>181</v>
       </c>
       <c r="D59">
@@ -3129,21 +3993,36 @@
       <c r="E59" t="s">
         <v>180</v>
       </c>
-      <c r="F59" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="G59" s="21" t="s">
+      <c r="F59" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="G59" s="20" t="s">
         <v>156</v>
       </c>
-      <c r="H59" s="23" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A60" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="C60" s="22" t="s">
+      <c r="H59" s="22" t="s">
+        <v>183</v>
+      </c>
+      <c r="J59" t="s">
+        <v>184</v>
+      </c>
+      <c r="K59" s="20" t="s">
+        <v>156</v>
+      </c>
+      <c r="L59" t="s">
+        <v>185</v>
+      </c>
+      <c r="M59" s="20" t="s">
+        <v>156</v>
+      </c>
+      <c r="N59" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="60" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A60" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="C60" s="21" t="s">
         <v>181</v>
       </c>
       <c r="D60">
@@ -3152,21 +4031,36 @@
       <c r="E60" t="s">
         <v>180</v>
       </c>
-      <c r="F60" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="G60" s="21" t="s">
+      <c r="F60" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="G60" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="H60" s="23" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A61" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="C61" s="22" t="s">
+      <c r="H60" s="22" t="s">
+        <v>183</v>
+      </c>
+      <c r="J60" t="s">
+        <v>184</v>
+      </c>
+      <c r="K60" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="L60" t="s">
+        <v>185</v>
+      </c>
+      <c r="M60" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="N60" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A61" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="C61" s="21" t="s">
         <v>181</v>
       </c>
       <c r="D61">
@@ -3175,21 +4069,36 @@
       <c r="E61" t="s">
         <v>180</v>
       </c>
-      <c r="F61" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="G61" s="21" t="s">
+      <c r="F61" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="G61" s="20" t="s">
         <v>157</v>
       </c>
-      <c r="H61" s="23" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="62" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A62" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="C62" s="22" t="s">
+      <c r="H61" s="22" t="s">
+        <v>183</v>
+      </c>
+      <c r="J61" t="s">
+        <v>184</v>
+      </c>
+      <c r="K61" s="20" t="s">
+        <v>157</v>
+      </c>
+      <c r="L61" t="s">
+        <v>185</v>
+      </c>
+      <c r="M61" s="20" t="s">
+        <v>157</v>
+      </c>
+      <c r="N61" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="62" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A62" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="C62" s="21" t="s">
         <v>181</v>
       </c>
       <c r="D62">
@@ -3198,21 +4107,36 @@
       <c r="E62" t="s">
         <v>180</v>
       </c>
-      <c r="F62" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="G62" s="21" t="s">
+      <c r="F62" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="G62" s="20" t="s">
         <v>158</v>
       </c>
-      <c r="H62" s="23" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="63" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A63" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="C63" s="22" t="s">
+      <c r="H62" s="22" t="s">
+        <v>183</v>
+      </c>
+      <c r="J62" t="s">
+        <v>184</v>
+      </c>
+      <c r="K62" s="20" t="s">
+        <v>158</v>
+      </c>
+      <c r="L62" t="s">
+        <v>185</v>
+      </c>
+      <c r="M62" s="20" t="s">
+        <v>158</v>
+      </c>
+      <c r="N62" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="63" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A63" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="C63" s="21" t="s">
         <v>181</v>
       </c>
       <c r="D63">
@@ -3221,21 +4145,36 @@
       <c r="E63" t="s">
         <v>180</v>
       </c>
-      <c r="F63" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="G63" s="21" t="s">
+      <c r="F63" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="G63" s="20" t="s">
         <v>159</v>
       </c>
-      <c r="H63" s="23" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A64" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="C64" s="22" t="s">
+      <c r="H63" s="22" t="s">
+        <v>183</v>
+      </c>
+      <c r="J63" t="s">
+        <v>184</v>
+      </c>
+      <c r="K63" s="20" t="s">
+        <v>159</v>
+      </c>
+      <c r="L63" t="s">
+        <v>185</v>
+      </c>
+      <c r="M63" s="20" t="s">
+        <v>159</v>
+      </c>
+      <c r="N63" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="64" spans="1:14" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A64" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="C64" s="21" t="s">
         <v>181</v>
       </c>
       <c r="D64">
@@ -3244,21 +4183,36 @@
       <c r="E64" t="s">
         <v>180</v>
       </c>
-      <c r="F64" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="G64" s="21" t="s">
+      <c r="F64" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="G64" s="20" t="s">
         <v>160</v>
       </c>
-      <c r="H64" s="23" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="65" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A65" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="C65" s="22" t="s">
+      <c r="H64" s="22" t="s">
+        <v>183</v>
+      </c>
+      <c r="J64" t="s">
+        <v>184</v>
+      </c>
+      <c r="K64" s="20" t="s">
+        <v>160</v>
+      </c>
+      <c r="L64" t="s">
+        <v>185</v>
+      </c>
+      <c r="M64" s="20" t="s">
+        <v>160</v>
+      </c>
+      <c r="N64" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="65" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A65" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="C65" s="21" t="s">
         <v>181</v>
       </c>
       <c r="D65">
@@ -3267,21 +4221,36 @@
       <c r="E65" t="s">
         <v>180</v>
       </c>
-      <c r="F65" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="G65" s="21" t="s">
+      <c r="F65" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="G65" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="H65" s="23" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="66" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A66" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="C66" s="22" t="s">
+      <c r="H65" s="22" t="s">
+        <v>183</v>
+      </c>
+      <c r="J65" t="s">
+        <v>184</v>
+      </c>
+      <c r="K65" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="L65" t="s">
+        <v>185</v>
+      </c>
+      <c r="M65" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="N65" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="66" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A66" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="C66" s="21" t="s">
         <v>181</v>
       </c>
       <c r="D66">
@@ -3290,21 +4259,36 @@
       <c r="E66" t="s">
         <v>180</v>
       </c>
-      <c r="F66" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="G66" s="21" t="s">
+      <c r="F66" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="G66" s="20" t="s">
         <v>161</v>
       </c>
-      <c r="H66" s="23" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="67" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A67" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="C67" s="22" t="s">
+      <c r="H66" s="22" t="s">
+        <v>183</v>
+      </c>
+      <c r="J66" t="s">
+        <v>184</v>
+      </c>
+      <c r="K66" s="20" t="s">
+        <v>161</v>
+      </c>
+      <c r="L66" t="s">
+        <v>185</v>
+      </c>
+      <c r="M66" s="20" t="s">
+        <v>161</v>
+      </c>
+      <c r="N66" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="67" spans="1:14" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A67" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="C67" s="21" t="s">
         <v>181</v>
       </c>
       <c r="D67">
@@ -3313,21 +4297,36 @@
       <c r="E67" t="s">
         <v>180</v>
       </c>
-      <c r="F67" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="G67" s="21" t="s">
+      <c r="F67" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="G67" s="20" t="s">
         <v>162</v>
       </c>
-      <c r="H67" s="23" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="68" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A68" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="C68" s="22" t="s">
+      <c r="H67" s="22" t="s">
+        <v>183</v>
+      </c>
+      <c r="J67" t="s">
+        <v>184</v>
+      </c>
+      <c r="K67" s="20" t="s">
+        <v>162</v>
+      </c>
+      <c r="L67" t="s">
+        <v>185</v>
+      </c>
+      <c r="M67" s="20" t="s">
+        <v>162</v>
+      </c>
+      <c r="N67" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="68" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A68" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="C68" s="21" t="s">
         <v>181</v>
       </c>
       <c r="D68">
@@ -3336,21 +4335,36 @@
       <c r="E68" t="s">
         <v>180</v>
       </c>
-      <c r="F68" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="G68" s="21" t="s">
+      <c r="F68" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="G68" s="20" t="s">
         <v>163</v>
       </c>
-      <c r="H68" s="23" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="69" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A69" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="C69" s="22" t="s">
+      <c r="H68" s="22" t="s">
+        <v>183</v>
+      </c>
+      <c r="J68" t="s">
+        <v>184</v>
+      </c>
+      <c r="K68" s="20" t="s">
+        <v>163</v>
+      </c>
+      <c r="L68" t="s">
+        <v>185</v>
+      </c>
+      <c r="M68" s="20" t="s">
+        <v>163</v>
+      </c>
+      <c r="N68" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="69" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A69" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="C69" s="21" t="s">
         <v>181</v>
       </c>
       <c r="D69">
@@ -3359,21 +4373,36 @@
       <c r="E69" t="s">
         <v>180</v>
       </c>
-      <c r="F69" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="G69" s="21" t="s">
+      <c r="F69" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="G69" s="20" t="s">
         <v>169</v>
       </c>
-      <c r="H69" s="23" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="70" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A70" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="C70" s="22" t="s">
+      <c r="H69" s="22" t="s">
+        <v>183</v>
+      </c>
+      <c r="J69" t="s">
+        <v>184</v>
+      </c>
+      <c r="K69" s="20" t="s">
+        <v>169</v>
+      </c>
+      <c r="L69" t="s">
+        <v>185</v>
+      </c>
+      <c r="M69" s="20" t="s">
+        <v>169</v>
+      </c>
+      <c r="N69" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="70" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A70" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="C70" s="21" t="s">
         <v>181</v>
       </c>
       <c r="D70">
@@ -3382,21 +4411,36 @@
       <c r="E70" t="s">
         <v>180</v>
       </c>
-      <c r="F70" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="G70" s="21" t="s">
+      <c r="F70" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="G70" s="20" t="s">
         <v>166</v>
       </c>
-      <c r="H70" s="23" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="71" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A71" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="C71" s="22" t="s">
+      <c r="H70" s="22" t="s">
+        <v>183</v>
+      </c>
+      <c r="J70" t="s">
+        <v>184</v>
+      </c>
+      <c r="K70" s="20" t="s">
+        <v>166</v>
+      </c>
+      <c r="L70" t="s">
+        <v>185</v>
+      </c>
+      <c r="M70" s="20" t="s">
+        <v>166</v>
+      </c>
+      <c r="N70" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="71" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A71" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="C71" s="21" t="s">
         <v>181</v>
       </c>
       <c r="D71">
@@ -3405,21 +4449,36 @@
       <c r="E71" t="s">
         <v>180</v>
       </c>
-      <c r="F71" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="G71" s="21" t="s">
+      <c r="F71" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="G71" s="20" t="s">
         <v>165</v>
       </c>
-      <c r="H71" s="23" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="72" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A72" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="C72" s="22" t="s">
+      <c r="H71" s="22" t="s">
+        <v>183</v>
+      </c>
+      <c r="J71" t="s">
+        <v>184</v>
+      </c>
+      <c r="K71" s="20" t="s">
+        <v>165</v>
+      </c>
+      <c r="L71" t="s">
+        <v>185</v>
+      </c>
+      <c r="M71" s="20" t="s">
+        <v>165</v>
+      </c>
+      <c r="N71" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="72" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A72" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="C72" s="21" t="s">
         <v>181</v>
       </c>
       <c r="D72">
@@ -3428,21 +4487,36 @@
       <c r="E72" t="s">
         <v>180</v>
       </c>
-      <c r="F72" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="G72" s="21" t="s">
+      <c r="F72" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="G72" s="20" t="s">
         <v>167</v>
       </c>
-      <c r="H72" s="23" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="73" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A73" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="C73" s="22" t="s">
+      <c r="H72" s="22" t="s">
+        <v>183</v>
+      </c>
+      <c r="J72" t="s">
+        <v>184</v>
+      </c>
+      <c r="K72" s="20" t="s">
+        <v>167</v>
+      </c>
+      <c r="L72" t="s">
+        <v>185</v>
+      </c>
+      <c r="M72" s="20" t="s">
+        <v>167</v>
+      </c>
+      <c r="N72" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="73" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A73" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="C73" s="21" t="s">
         <v>181</v>
       </c>
       <c r="D73">
@@ -3451,21 +4525,36 @@
       <c r="E73" t="s">
         <v>180</v>
       </c>
-      <c r="F73" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="G73" s="21" t="s">
+      <c r="F73" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="G73" s="20" t="s">
         <v>168</v>
       </c>
-      <c r="H73" s="23" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="74" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A74" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="C74" s="22" t="s">
+      <c r="H73" s="22" t="s">
+        <v>183</v>
+      </c>
+      <c r="J73" t="s">
+        <v>184</v>
+      </c>
+      <c r="K73" s="20" t="s">
+        <v>168</v>
+      </c>
+      <c r="L73" t="s">
+        <v>185</v>
+      </c>
+      <c r="M73" s="20" t="s">
+        <v>168</v>
+      </c>
+      <c r="N73" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="74" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A74" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="C74" s="21" t="s">
         <v>181</v>
       </c>
       <c r="D74">
@@ -3474,14 +4563,29 @@
       <c r="E74" t="s">
         <v>180</v>
       </c>
-      <c r="F74" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="G74" s="21" t="s">
+      <c r="F74" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="G74" s="20" t="s">
         <v>56</v>
       </c>
-      <c r="H74" s="23" t="s">
-        <v>183</v>
+      <c r="H74" s="22" t="s">
+        <v>183</v>
+      </c>
+      <c r="J74" t="s">
+        <v>184</v>
+      </c>
+      <c r="K74" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="L74" t="s">
+        <v>185</v>
+      </c>
+      <c r="M74" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="N74" t="s">
+        <v>186</v>
       </c>
     </row>
   </sheetData>

</xml_diff>